<commit_message>
Cambios del correo del 16 de feb
</commit_message>
<xml_diff>
--- a/xlsx/a69_f21_bUPPachuca.xlsx
+++ b/xlsx/a69_f21_bUPPachuca.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\Vo.Bo. Uno UPP 4T 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\SIPOT 4TO TRIMESTRE\Fracciones con Cierre Trimestral 4to 2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
     <sheet name="Tabla_393859" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>46582</t>
   </si>
@@ -179,14 +179,29 @@
     <t>Subdirección de Planeación y Presupuesto (UPP)</t>
   </si>
   <si>
-    <t>Derivado del Cierre financiero - presupuestal que se trabaja de manera  coordinada entre planeación y administración para la entrega y preparación de información ante las diversas dependencias fiscalizadoras , en apego al artículo 15 de la ley de fiscalización superior y rendición de cuenta de estado de hidalgo,  correlativamente con la fracción v del artículo 28 de la misma ley se establecen como fecha de entrega  los siete días hábiles siguientes al cierre del trimestre.  Así también dentro del convenio especifico para la  asignación de recursos con carácter de apoyo solidario firmado entre la federación y el estado en su cláusula sexta fracción "f" donde obliga la entrega de los estados financieros dentro de los primeros diez días hábiles a la coordinación de universidades tecnológicas y politécnicas. Motivo por el cual estaremos entregando la información con cifras definitivas, el 28 de enero del año en curso.</t>
+    <t>Servicios Personales</t>
+  </si>
+  <si>
+    <t>Materiales y Suministros</t>
+  </si>
+  <si>
+    <t>Servicios Generales</t>
+  </si>
+  <si>
+    <t>Transferencia, Asignaciones, Subsidios y Otras Ayudas</t>
+  </si>
+  <si>
+    <t>Bienes Muebles, Inmuebles e Intangibles</t>
+  </si>
+  <si>
+    <t>http://www.upp.edu.mx/leygralcontabilidad/mc/02-edospres/05-informacion-presupuestaria/2020/a_diciembre_2020/06.estadoanaliticopresupuestoegresos-cap-gto_ex.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -206,6 +221,14 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -250,24 +273,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -278,14 +299,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,11 +598,11 @@
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.85546875" customWidth="1"/>
     <col min="6" max="6" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="85.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -589,38 +611,38 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -681,71 +703,73 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>2020</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>44105</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>44196</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3" t="s">
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>44206</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>44206</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="I8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -757,17 +781,19 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,32 +862,177 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="3">
+        <v>29464300</v>
+      </c>
+      <c r="E4" s="3">
+        <v>9500937.799999997</v>
+      </c>
+      <c r="F4" s="3">
+        <v>38965237.799999997</v>
+      </c>
+      <c r="G4" s="3">
+        <v>38965237.799999997</v>
+      </c>
+      <c r="H4" s="3">
+        <v>38965237.799999997</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="3">
+        <v>446688</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1764496.92</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2211184.92</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2211184.92</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2711184.92</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="3">
+        <v>8823562</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-3531843.7199999997</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5291718.28</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5291718.28</v>
+      </c>
+      <c r="H6" s="3">
+        <v>5205483.99</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4000</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="3">
+        <v>241025</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-241025</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5000</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>55100</v>
+      </c>
+      <c r="F8" s="4">
+        <v>55100</v>
+      </c>
+      <c r="G8" s="4">
+        <v>55100</v>
+      </c>
+      <c r="H8" s="4">
+        <v>55100</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios para las 11
</commit_message>
<xml_diff>
--- a/xlsx/a69_f21_bUPPachuca.xlsx
+++ b/xlsx/a69_f21_bUPPachuca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\2do Trimestre SIPOT 2021\2do Trimestre UPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\CIERRE PRESUPUESTAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>46582</t>
   </si>
@@ -179,14 +179,29 @@
     <t>Subdirección de Planeación y Presupuesto (UPP)</t>
   </si>
   <si>
-    <t>Derivado del Cierre financiero - presupuestal que se trabaja de manera  coordinada entre planeación y administración para la entrega y preparación de información ante las diversas dependencias fiscalizadoras , en apego al artículo 15 de la ley de fiscalización superior y rendición de cuenta de estado de hidalgo,  correlativamente con la fracción V del artículo 28 de la misma ley se establecen como fecha de entrega  los siete días hábiles siguientes al cierre del trimestre.  Así también dentro del convenio especifico para la  asignación de recursos con carácter de apoyo solidario firmado entre la federación y el estado en su cláusula sexta fracción "f" donde obliga la entrega de los estados financieros dentro de los primeros diez días hábiles a la coordinación de universidades tecnológicas y politécnicas. Motivo por el cual estaremos entregando la información con cifras definitivas, el 26 de julio del año en curso</t>
+    <t>Servicios Personales</t>
+  </si>
+  <si>
+    <t>Materiales y Suministros</t>
+  </si>
+  <si>
+    <t>Servicios Generales</t>
+  </si>
+  <si>
+    <t>Transferencia, Asignaciones, Subsidios y Otras Ayudas</t>
+  </si>
+  <si>
+    <t>Bienes Muebles, Inmuebles e Intangibles</t>
+  </si>
+  <si>
+    <t>http://www.upp.edu.mx/leygralcontabilidad/mc/02-edospres/05-informacion-presupuestaria/2021/a_junio_2021/06.estadoanaliticopresupuestoegresos-cap-gto_ex.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -206,6 +221,14 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -250,10 +273,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -265,27 +289,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,11 +604,11 @@
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="161.5703125" customWidth="1"/>
+    <col min="6" max="6" width="73.42578125" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="80.5703125" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -589,38 +617,38 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -681,17 +709,17 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -722,8 +750,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>2021</v>
       </c>
       <c r="B8" s="3">
@@ -732,9 +760,13 @@
       <c r="C8" s="3">
         <v>44377</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6" t="s">
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>51</v>
       </c>
       <c r="G8" s="3">
@@ -743,9 +775,7 @@
       <c r="H8" s="3">
         <v>44386</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="I8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -757,17 +787,19 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,6 +896,151 @@
         <v>50</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="8">
+        <v>48094261</v>
+      </c>
+      <c r="E4" s="8">
+        <v>-953512.67000000179</v>
+      </c>
+      <c r="F4" s="8">
+        <v>47140748.329999998</v>
+      </c>
+      <c r="G4" s="8">
+        <v>47140748.329999998</v>
+      </c>
+      <c r="H4" s="8">
+        <v>47140748.329999998</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1410534</v>
+      </c>
+      <c r="E5" s="8">
+        <v>-957349.91999999993</v>
+      </c>
+      <c r="F5" s="8">
+        <v>453184.08</v>
+      </c>
+      <c r="G5" s="8">
+        <v>453184.08</v>
+      </c>
+      <c r="H5" s="8">
+        <v>453184.08</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="8">
+        <v>6392543</v>
+      </c>
+      <c r="E6" s="8">
+        <v>-1945783.79</v>
+      </c>
+      <c r="F6" s="8">
+        <v>4446759.21</v>
+      </c>
+      <c r="G6" s="8">
+        <v>4446759.21</v>
+      </c>
+      <c r="H6" s="8">
+        <v>4446759.21</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
+        <v>4000</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="8">
+        <v>53200</v>
+      </c>
+      <c r="E7" s="8">
+        <v>-42006</v>
+      </c>
+      <c r="F7" s="8">
+        <v>11194</v>
+      </c>
+      <c r="G7" s="8">
+        <v>11194</v>
+      </c>
+      <c r="H7" s="8">
+        <v>11194</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8">
+        <v>5000</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="8">
+        <v>736000</v>
+      </c>
+      <c r="E8" s="8">
+        <v>-537232</v>
+      </c>
+      <c r="F8" s="8">
+        <v>198768</v>
+      </c>
+      <c r="G8" s="8">
+        <v>198768</v>
+      </c>
+      <c r="H8" s="8">
+        <v>198768</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
archivos con errores del 10 de dic
</commit_message>
<xml_diff>
--- a/xlsx/a69_f21_bUPPachuca.xlsx
+++ b/xlsx/a69_f21_bUPPachuca.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\SIPOT 3ER TRIMETRES 2021\UPP 3ER TRIMESTRE 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\SIPOT 3ER TRIMETRES 2021\UPP Fracciones con Cierre Presupuestal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7065"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
     <sheet name="Tabla_393859" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>46582</t>
   </si>
@@ -179,14 +179,29 @@
     <t>Subdirección de Planeación y Presupuesto (UPP)</t>
   </si>
   <si>
-    <t>Derivado del Cierre financiero - presupuestal que se trabaja de manera  coordinada entre planeación y administración para la entrega y preparación de información ante las diversas dependencias fiscalizadoras , en apego al artículo 15 de la ley de fiscalización superior y rendición de cuenta de estado de hidalgo,  correlativamente con la fracción V del artículo 28 de la misma ley se establecen como fecha de entrega  los siete días hábiles siguientes al cierre del trimestre.  Así también dentro del convenio especifico para la  asignación de recursos con carácter de apoyo solidario firmado entre la federación y el estado en su cláusula sexta fracción "f" donde obliga la entrega de los estados financieros dentro de los primeros diez días hábiles a la coordinación de universidades tecnológicas y politécnicas. Motivo por el cual estaremos entregando la información con cifras definitivas, el 27 de octubre del año en curso.</t>
+    <t>Servicios Personales</t>
+  </si>
+  <si>
+    <t>Materiales y Suministros</t>
+  </si>
+  <si>
+    <t>Servicios Generales</t>
+  </si>
+  <si>
+    <t>Transferencia, Asignaciones, Subsidios y Otras Ayudas</t>
+  </si>
+  <si>
+    <t>Bienes Muebles, Inmuebles e Intangibles</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/leygralcontabilidad/mc/02-edospres/05-informacion-presupuestaria/2021/a_septiembre_2021/06.estadoanaliticopresupuestoegresos-cap-gto_ex.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -206,6 +221,14 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -250,10 +273,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -261,6 +285,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -269,9 +294,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -284,8 +306,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,11 +602,11 @@
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="111" customWidth="1"/>
     <col min="6" max="6" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="83" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -605,7 +631,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -651,7 +677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -722,30 +748,32 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>2021</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>44378</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>44469</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="5">
         <v>44480</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="5">
         <v>44480</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="I8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -757,29 +785,32 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -864,6 +895,151 @@
         <v>50</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="4">
+        <v>75416997</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-2042402.1200000048</v>
+      </c>
+      <c r="F4" s="4">
+        <v>73374594.879999995</v>
+      </c>
+      <c r="G4" s="4">
+        <v>73374594.879999995</v>
+      </c>
+      <c r="H4" s="4">
+        <v>73374594.879999995</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1715034</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-977449.3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>737584.7</v>
+      </c>
+      <c r="G5" s="4">
+        <v>737584.7</v>
+      </c>
+      <c r="H5" s="4">
+        <v>737584.7</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="4">
+        <v>9157271</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-1890478.13</v>
+      </c>
+      <c r="F6" s="4">
+        <v>7266792.8700000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>7266792.8700000001</v>
+      </c>
+      <c r="H6" s="4">
+        <v>7258793.1300000008</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4000</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="4">
+        <v>84000</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-72806</v>
+      </c>
+      <c r="F7" s="4">
+        <v>11194</v>
+      </c>
+      <c r="G7" s="4">
+        <v>11194</v>
+      </c>
+      <c r="H7" s="4">
+        <v>11194</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="4">
+        <v>736000</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-537232</v>
+      </c>
+      <c r="F8" s="4">
+        <v>198768</v>
+      </c>
+      <c r="G8" s="4">
+        <v>198768</v>
+      </c>
+      <c r="H8" s="4">
+        <v>198768</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios incompletos de maydeli
</commit_message>
<xml_diff>
--- a/xlsx/a69_f21_bUPPachuca.xlsx
+++ b/xlsx/a69_f21_bUPPachuca.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maydeli\Documents\TRANSPARENCIA\UPP Cierre Presupuestal 2do Tri 2022\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
     <sheet name="Tabla_393859" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>46582</t>
   </si>
@@ -174,14 +191,29 @@
     <t>Subdirección de Planeación y Presupuesto (UPP)</t>
   </si>
   <si>
-    <t>La información solicitada se entregará a más tardar el día 30 de julio del años en curso en terminos del art.58 de la Ley General de Contabilidad Gubernamental.</t>
+    <t>Servicios Personales</t>
+  </si>
+  <si>
+    <t>Materiales y Suministros</t>
+  </si>
+  <si>
+    <t>Servicios Generales</t>
+  </si>
+  <si>
+    <t>Transferencia, Asignaciones, Subsidios y Otras Ayudas</t>
+  </si>
+  <si>
+    <t>Bienes Muebles, Inmuebles e Intangibles</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/leygralcontabilidad/mc/02-edospres/05-informacion-presupuestaria/2022/a_junio_2022/11.estadoanaliticopresupuestoegresos.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -209,6 +241,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -228,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -251,20 +291,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -284,17 +316,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -353,7 +383,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +418,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -599,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,11 +639,11 @@
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.5703125" customWidth="1"/>
     <col min="6" max="6" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.140625" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -638,7 +668,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -649,11 +679,11 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -755,7 +785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2022</v>
       </c>
@@ -765,8 +795,12 @@
       <c r="C8" s="4">
         <v>44742</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="F8" s="5" t="s">
         <v>51</v>
       </c>
@@ -776,9 +810,7 @@
       <c r="H8" s="4">
         <v>44753</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>52</v>
-      </c>
+      <c r="I8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -790,22 +822,26 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -895,6 +931,157 @@
         <v>50</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="3">
+        <v>55738372</v>
+      </c>
+      <c r="E4" s="3">
+        <f>F4-D4</f>
+        <v>-7835940.0700000003</v>
+      </c>
+      <c r="F4" s="3">
+        <v>47902431.93</v>
+      </c>
+      <c r="G4" s="3">
+        <v>47902431.93</v>
+      </c>
+      <c r="H4" s="3">
+        <v>47902431.93</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2078468</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E8" si="0">F5-D5</f>
+        <v>-1563478.94</v>
+      </c>
+      <c r="F5" s="3">
+        <v>514989.06</v>
+      </c>
+      <c r="G5" s="3">
+        <v>514989.06</v>
+      </c>
+      <c r="H5" s="3">
+        <v>514989.06</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7114245</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>-1509775.1500000004</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5604469.8499999996</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5604469.8499999996</v>
+      </c>
+      <c r="H6" s="3">
+        <v>5604469.8499999996</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4000</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="3">
+        <f>4544024.58-1711058.58</f>
+        <v>2832966</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>-2832966</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5000</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1675330</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>-1455330</v>
+      </c>
+      <c r="F8" s="3">
+        <v>220000</v>
+      </c>
+      <c r="G8" s="3">
+        <v>220000</v>
+      </c>
+      <c r="H8" s="3">
+        <v>220000</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>